<commit_message>
powiar rw + zlacze baterii
koniecznie sprawdzić masy i flagi
</commit_message>
<xml_diff>
--- a/zakupy.xlsx
+++ b/zakupy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piate\Documents\GitHub\Universal_charger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B88B221-E0CF-4F69-800D-97A08F631B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580D7AC6-FE3E-4BF2-9CED-86D9520A70BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <t>symbol</t>
   </si>
@@ -251,6 +251,27 @@
   </si>
   <si>
     <t>https://www.tme.eu/Document/75af175f80c090e9b8f9078a0b0b2409/ACS712.PDF</t>
+  </si>
+  <si>
+    <t>AO4425</t>
+  </si>
+  <si>
+    <t>p mos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r 100k </t>
+  </si>
+  <si>
+    <t>c 1n</t>
+  </si>
+  <si>
+    <t>c 100n</t>
+  </si>
+  <si>
+    <t>złącze bateri XC90?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">przejrzeć masy i flagi </t>
   </si>
 </sst>
 </file>
@@ -260,7 +281,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +310,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,11 +341,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -1117,12 +1147,12 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="14.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.07421875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.07421875" bestFit="1" customWidth="1"/>
@@ -1207,11 +1237,11 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f>D3*4</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1330,11 +1360,11 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E10" si="0">D7*4</f>
-        <v>48</v>
+        <f t="shared" ref="E7:E12" si="0">D7*4</f>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>29</v>
@@ -1426,7 +1456,7 @@
       <c r="I10" t="s">
         <v>15</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1434,30 +1464,74 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
@@ -1540,6 +1614,7 @@
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{7C1CD807-B7DC-4ADB-8FE5-1357B658128E}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{797C5E85-882D-47F7-8433-D07ABAFD28D0}"/>
+    <hyperlink ref="J10" r:id="rId3" xr:uid="{4C9A6A05-4EE9-439D-8B6B-F0B73BC66D10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Skończone - do przejrzenia
</commit_message>
<xml_diff>
--- a/zakupy.xlsx
+++ b/zakupy.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="127">
   <si>
     <t>symbol</t>
   </si>
@@ -337,9 +337,6 @@
     <t>CA1E337M10010VR</t>
   </si>
   <si>
-    <t>cewka 47uH 10A</t>
-  </si>
-  <si>
     <t>rezystor 100</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
     <t>B540C-13-F</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>MiniMELF</t>
   </si>
   <si>
@@ -394,7 +388,37 @@
     <t>footprint na TME</t>
   </si>
   <si>
-    <t>0.14</t>
+    <t>? / 3220</t>
+  </si>
+  <si>
+    <t>DPU047A5</t>
+  </si>
+  <si>
+    <t>DPO-5.0-47</t>
+  </si>
+  <si>
+    <t>cewka 47uH 5A THD</t>
+  </si>
+  <si>
+    <t>trzeba stwierdzić czy 5A wystarczy (według noty przetwornicy tak)</t>
+  </si>
+  <si>
+    <t>Inductor_THT:L_Toroid_Vertical_L25.4mm_W14.7mm_P12.20mm_Vishay_TJ5</t>
+  </si>
+  <si>
+    <t>zamówiona partia z chin, najwyzej wylut z przetwornicy z allegro</t>
+  </si>
+  <si>
+    <t>imo lepiej smd</t>
+  </si>
+  <si>
+    <t>cewka 47uH 6.8A SMD</t>
+  </si>
+  <si>
+    <t>ETQP5M470YFC</t>
+  </si>
+  <si>
+    <t>Inductor_SMD:L_Bourns-SRN8040_8x8.15mm</t>
   </si>
 </sst>
 </file>
@@ -435,12 +459,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -457,12 +487,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -1852,21 +1884,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.28515625" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
@@ -1923,6 +1955,9 @@
       <c r="G2" s="4">
         <v>5</v>
       </c>
+      <c r="H2" t="s">
+        <v>122</v>
+      </c>
       <c r="I2" t="s">
         <v>95</v>
       </c>
@@ -1941,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E15" si="0">D3*4</f>
+        <f t="shared" ref="E3:E5" si="0">D3*4</f>
         <v>16</v>
       </c>
       <c r="F3" t="s">
@@ -1961,160 +1996,177 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3.11</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1.53</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F5" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="I5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>116</v>
+      <c r="G5" s="6">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
         <v>112</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>D6*4</f>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>118</v>
+      <c r="G6" s="4">
+        <v>1.53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f>D7*4</f>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="G7" s="4">
-        <v>0.42</v>
-      </c>
-      <c r="I7">
-        <v>805</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I7" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>D8*4</f>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="I8" t="s">
-        <v>96</v>
+        <v>0.42</v>
+      </c>
+      <c r="I8">
+        <v>805</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>D9*4</f>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="G9" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="I9">
-        <v>805</v>
+        <v>0.95</v>
+      </c>
+      <c r="I9" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>D10*4</f>
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="G10" s="4">
         <v>0.06</v>
@@ -2125,20 +2177,20 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>D11*4</f>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G11" s="4">
         <v>0.06</v>
@@ -2149,20 +2201,20 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>D12*4</f>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G12" s="4">
         <v>0.06</v>
@@ -2173,23 +2225,23 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>D13*4</f>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G13" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="I13">
         <v>805</v>
@@ -2197,7 +2249,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
         <v>110</v>
@@ -2206,14 +2258,14 @@
         <v>2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>D14*4</f>
         <v>8</v>
       </c>
       <c r="F14" t="s">
         <v>110</v>
       </c>
       <c r="G14" s="4">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I14">
         <v>805</v>
@@ -2221,25 +2273,49 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>D15*4</f>
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G15" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="I15">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f>D16*4</f>
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>805</v>
       </c>
     </row>
@@ -2247,7 +2323,7 @@
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1"/>
     <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J5" r:id="rId3"/>
+    <hyperlink ref="J6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Updated buy list with mcu components
</commit_message>
<xml_diff>
--- a/zakupy.xlsx
+++ b/zakupy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piate\Documents\GitHub\Universal_charger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\btlf\OneDrive\Documents\GitHub\Universal_charger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C854324-828C-441F-B504-8F081F452027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F676E6FC-6452-46B1-9DA5-31544663BDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2477" yWindow="1817" windowWidth="16372" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wszystko" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="164">
   <si>
     <t>symbol</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>SRN8040_8x8.15mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mux </t>
+  </si>
+  <si>
+    <t>CD74HC4051M</t>
+  </si>
+  <si>
+    <t>SO16</t>
   </si>
 </sst>
 </file>
@@ -675,15 +684,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>658586</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>39461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>5355157</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>5326582</xdr:colOff>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>96872</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -707,8 +716,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10316936" y="6554561"/>
-          <a:ext cx="5344271" cy="1867161"/>
+          <a:off x="10497911" y="8040461"/>
+          <a:ext cx="5344271" cy="1962411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1122,23 +1131,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.07421875" customWidth="1"/>
-    <col min="10" max="10" width="123.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="123.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G36" si="0">D2*4</f>
+        <f t="shared" ref="G2:G38" si="0">D2*4</f>
         <v>24</v>
       </c>
       <c r="I2" s="13" t="s">
@@ -1188,7 +1197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1243,7 +1252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1279,21 +1288,21 @@
         <v>27</v>
       </c>
       <c r="D6">
-        <f>12+3+1+4</f>
-        <v>20</v>
+        <f>12+3+1+4+4</f>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>29</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="I6" s="13">
         <v>805</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1304,21 +1313,21 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <f>6+8+5</f>
-        <v>19</v>
+        <f>6+8+5+3</f>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>32</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I7" s="13">
         <v>805</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1343,7 +1352,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1367,7 +1376,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1391,7 +1400,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1415,7 +1424,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1426,21 +1435,21 @@
         <v>47</v>
       </c>
       <c r="D12">
-        <f>6+4+4+2</f>
-        <v>16</v>
+        <f>6+4+4+2+2</f>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
         <v>48</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="I12" s="13">
         <v>805</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1465,7 +1474,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1544,7 +1553,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1570,7 +1579,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1597,7 +1606,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1649,7 +1658,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1677,7 +1686,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1702,7 +1711,7 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1750,7 +1759,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1774,7 +1783,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1801,7 +1810,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1825,7 +1834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1849,7 +1858,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1897,7 +1906,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1921,7 +1930,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1946,7 +1955,7 @@
       </c>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1998,7 +2007,7 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2009,21 +2018,22 @@
         <v>97</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <f>6+4</f>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
         <v>97</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="I35">
         <v>805</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2051,28 +2061,47 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>162</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="J40" s="11"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2109,20 +2138,20 @@
       <selection activeCell="J2" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.69140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.53515625" customWidth="1"/>
-    <col min="7" max="7" width="6.53515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.15234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="123.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="123.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2154,7 +2183,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2187,7 +2216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2220,7 +2249,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2253,7 +2282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2281,7 +2310,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2309,7 +2338,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2337,7 +2366,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2365,7 +2394,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2393,7 +2422,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2421,7 +2450,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2449,7 +2478,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2480,115 +2509,115 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2609,22 +2638,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="76.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="76.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2689,7 +2718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2722,7 +2751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2752,7 +2781,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2782,7 +2811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2812,7 +2841,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2839,7 +2868,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2866,7 +2895,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2893,7 +2922,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2923,7 +2952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2950,7 +2979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2977,7 +3006,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3007,7 +3036,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3037,7 +3066,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3067,7 +3096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3076,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3085,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3094,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3124,62 +3153,62 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3204,22 +3233,22 @@
       <selection activeCell="B2" sqref="B2:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="19.84375" customWidth="1"/>
-    <col min="5" max="5" width="19.15234375" customWidth="1"/>
-    <col min="6" max="6" width="18.3828125" customWidth="1"/>
-    <col min="7" max="7" width="18.3046875" customWidth="1"/>
-    <col min="8" max="8" width="59.3046875" customWidth="1"/>
-    <col min="9" max="9" width="10.15234375" customWidth="1"/>
-    <col min="10" max="10" width="16.3046875" customWidth="1"/>
-    <col min="11" max="11" width="20.84375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="59.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3251,7 +3280,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>88</v>
       </c>
@@ -3281,7 +3310,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>51</v>
       </c>
@@ -3311,7 +3340,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3338,7 +3367,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>119</v>
       </c>
@@ -3365,7 +3394,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>90</v>
       </c>
@@ -3395,7 +3424,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>91</v>
       </c>
@@ -3419,7 +3448,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>92</v>
       </c>
@@ -3443,7 +3472,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>93</v>
       </c>
@@ -3477,7 +3506,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>99</v>
       </c>
@@ -3501,7 +3530,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>100</v>
       </c>
@@ -3525,7 +3554,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>101</v>
       </c>
@@ -3549,7 +3578,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>102</v>
       </c>
@@ -3573,7 +3602,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>103</v>
       </c>
@@ -3597,7 +3626,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>104</v>
       </c>
@@ -3621,7 +3650,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>105</v>
       </c>
@@ -3664,9 +3693,9 @@
       <selection activeCell="B2" sqref="B2:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3698,7 +3727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3728,7 +3757,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -3757,7 +3786,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -3786,7 +3815,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -3812,7 +3841,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -3838,7 +3867,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3867,7 +3896,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3896,7 +3925,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3922,7 +3951,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3948,27 +3977,27 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>